<commit_message>
new try to order tasks
</commit_message>
<xml_diff>
--- a/.tasks/TaskJuggle.xlsx
+++ b/.tasks/TaskJuggle.xlsx
@@ -8,7 +8,8 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Tasks juggle" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Repeated Tasks" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="45">
   <si>
     <t xml:space="preserve">Category</t>
   </si>
@@ -103,10 +104,16 @@
 </t>
   </si>
   <si>
+    <t xml:space="preserve">change log.php</t>
+  </si>
+  <si>
     <t xml:space="preserve">6
 </t>
   </si>
   <si>
+    <t xml:space="preserve">Doc / Clean code </t>
+  </si>
+  <si>
     <t xml:space="preserve">7
 </t>
   </si>
@@ -114,8 +121,14 @@
     <t xml:space="preserve">Release Ajax</t>
   </si>
   <si>
+    <t xml:space="preserve">User Doc</t>
+  </si>
+  <si>
     <t xml:space="preserve">8
 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Release →…</t>
   </si>
   <si>
     <t xml:space="preserve">9
@@ -308,7 +321,7 @@
   <dimension ref="A3:K23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
+      <selection pane="topLeft" activeCell="I12" activeCellId="0" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -408,102 +421,114 @@
       </c>
       <c r="F7" s="8"/>
     </row>
-    <row r="8" s="6" customFormat="true" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" s="6" customFormat="true" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="7" t="s">
         <v>24</v>
       </c>
       <c r="F8" s="8"/>
-    </row>
-    <row r="9" s="6" customFormat="true" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I8" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" s="6" customFormat="true" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F9" s="8"/>
+      <c r="I9" s="6" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="10" s="6" customFormat="true" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="7" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F10" s="8"/>
+      <c r="I10" s="6" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="11" s="6" customFormat="true" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="7" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="F11" s="8"/>
+      <c r="I11" s="0" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="12" s="6" customFormat="true" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="7" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="F12" s="8"/>
     </row>
     <row r="13" s="6" customFormat="true" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="7" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="F13" s="8"/>
     </row>
     <row r="14" s="6" customFormat="true" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="7" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="F14" s="8"/>
     </row>
     <row r="15" s="6" customFormat="true" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="7" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="F15" s="8"/>
     </row>
     <row r="16" s="6" customFormat="true" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="7" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="F16" s="8"/>
     </row>
     <row r="17" s="6" customFormat="true" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="7" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="F17" s="8"/>
     </row>
     <row r="18" s="6" customFormat="true" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="7" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="F18" s="8"/>
     </row>
     <row r="19" s="6" customFormat="true" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="7" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="F19" s="8"/>
     </row>
     <row r="20" s="6" customFormat="true" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="7" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="F20" s="8"/>
     </row>
     <row r="21" s="6" customFormat="true" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="7" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="F21" s="8"/>
     </row>
     <row r="22" s="6" customFormat="true" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="7" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="F22" s="8"/>
     </row>
     <row r="23" s="6" customFormat="true" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="7" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="F23" s="8"/>
     </row>
@@ -516,4 +541,46 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="B3:B5"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="19.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added tasks for Config move
</commit_message>
<xml_diff>
--- a/.tasks/TaskJuggle.xlsx
+++ b/.tasks/TaskJuggle.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="82">
   <si>
     <t xml:space="preserve">Category</t>
   </si>
@@ -69,13 +69,19 @@
     <t xml:space="preserve">Edit image → double click on image</t>
   </si>
   <si>
+    <t xml:space="preserve">Rename Maintenance “Consolidate image Database”</t>
+  </si>
+  <si>
     <t xml:space="preserve">Test FTP on server</t>
   </si>
   <si>
-    <t xml:space="preserve">New ICON , better Information pre/post ..
+    <t xml:space="preserve">New ICON , better Information pre/post 
 TaskInstall.170121 .png</t>
   </si>
   <si>
+    <t xml:space="preserve">Repair Zone: image Db first element</t>
+  </si>
+  <si>
     <t xml:space="preserve">b) Image editor </t>
   </si>
   <si>
@@ -92,12 +98,18 @@
     <t xml:space="preserve">On Drag/drop upload vertical images same size ==&gt; image Properties not</t>
   </si>
   <si>
+    <t xml:space="preserve">Check for single left over installation files</t>
+  </si>
+  <si>
     <t xml:space="preserve">Test zip on server</t>
   </si>
   <si>
     <t xml:space="preserve">Improve layout of user information -&gt; first install</t>
   </si>
   <si>
+    <t xml:space="preserve">Copy old to new configuration data ==&gt; Test</t>
+  </si>
+  <si>
     <t xml:space="preserve">a) After upload</t>
   </si>
   <si>
@@ -117,6 +129,9 @@
     <t xml:space="preserve">Improve layout of user information -&gt; update</t>
   </si>
   <si>
+    <t xml:space="preserve">Save and copy to old configuration data ==&gt; Test</t>
+  </si>
+  <si>
     <t xml:space="preserve">Tell new version → drag / drop</t>
   </si>
   <si>
@@ -127,6 +142,9 @@
     <t xml:space="preserve">Improve layout of user information -&gt; button for RSGallery2 jump on both update and install</t>
   </si>
   <si>
+    <t xml:space="preserve">Save to text file ==&gt; Test</t>
+  </si>
+  <si>
     <t xml:space="preserve">Update download links in forum</t>
   </si>
   <si>
@@ -134,10 +152,16 @@
 </t>
   </si>
   <si>
+    <t xml:space="preserve">Read from text file ==&gt; Test</t>
+  </si>
+  <si>
     <t xml:space="preserve">6
 </t>
   </si>
   <si>
+    <t xml:space="preserve">Save (old) and copy to new configuration data ==&gt; Test</t>
+  </si>
+  <si>
     <t xml:space="preserve">7
 </t>
   </si>
@@ -145,15 +169,24 @@
     <t xml:space="preserve">Release Ajax</t>
   </si>
   <si>
+    <t xml:space="preserve">Save (old) to text file</t>
+  </si>
+  <si>
     <t xml:space="preserve">8
 </t>
   </si>
   <si>
+    <t xml:space="preserve">Read (old) from text file ==&gt; Test</t>
+  </si>
+  <si>
     <t xml:space="preserve">Test on server</t>
   </si>
   <si>
     <t xml:space="preserve">9
 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">remove_OldConfigData ask for confirmation ==&gt; Test</t>
   </si>
   <si>
     <t xml:space="preserve">change log.php</t>
@@ -301,7 +334,7 @@
     </font>
     <font>
       <sz val="8"/>
-      <color rgb="FFCE181E"/>
+      <color rgb="FF0066B3"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -397,12 +430,12 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -446,7 +479,7 @@
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
-      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FF0066B3"/>
       <rgbColor rgb="FFCCCCFF"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
@@ -492,8 +525,8 @@
   </sheetPr>
   <dimension ref="A3:N23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -556,238 +589,269 @@
       <c r="C4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="6"/>
+      <c r="D4" s="6" t="s">
+        <v>15</v>
+      </c>
       <c r="E4" s="7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" s="8"/>
-      <c r="K4" s="9" t="s">
         <v>17</v>
       </c>
+      <c r="G4" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" s="9"/>
+      <c r="K4" s="8" t="s">
+        <v>19</v>
+      </c>
       <c r="L4" s="3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="N4" s="10" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" s="3" customFormat="true" ht="48.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="6" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>25</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="H5" s="8"/>
-      <c r="K5" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="L5" s="9"/>
+        <v>26</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" s="9"/>
+      <c r="K5" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="L5" s="8"/>
       <c r="N5" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" s="3" customFormat="true" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" s="3" customFormat="true" ht="38.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="6" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D6" s="6"/>
-      <c r="E6" s="3" t="s">
-        <v>28</v>
+      <c r="E6" s="8" t="s">
+        <v>32</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="H6" s="8"/>
+        <v>33</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H6" s="9"/>
       <c r="N6" s="3" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" s="3" customFormat="true" ht="57.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="6" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
       <c r="F7" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="H7" s="8"/>
+        <v>37</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H7" s="9"/>
       <c r="K7" s="0"/>
       <c r="L7" s="0"/>
       <c r="N7" s="3" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" s="3" customFormat="true" ht="29.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="6" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
       <c r="F8" s="0"/>
-      <c r="H8" s="8"/>
+      <c r="G8" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H8" s="9"/>
       <c r="K8" s="0"/>
       <c r="L8" s="0"/>
     </row>
-    <row r="9" s="3" customFormat="true" ht="29.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" s="3" customFormat="true" ht="38.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="6" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
       <c r="F9" s="0"/>
-      <c r="H9" s="8"/>
+      <c r="G9" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="H9" s="9"/>
       <c r="K9" s="0"/>
       <c r="L9" s="0"/>
     </row>
     <row r="10" s="3" customFormat="true" ht="29.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="6" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
       <c r="E10" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="H10" s="8"/>
+        <v>45</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H10" s="9"/>
       <c r="K10" s="0"/>
       <c r="L10" s="0"/>
     </row>
     <row r="11" s="3" customFormat="true" ht="29.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="6" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
-      <c r="H11" s="8"/>
-      <c r="K11" s="9" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" s="3" customFormat="true" ht="29.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G11" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="H11" s="9"/>
+      <c r="K11" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" s="3" customFormat="true" ht="38.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="6" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
-      <c r="H12" s="8"/>
-      <c r="K12" s="9" t="s">
-        <v>41</v>
+      <c r="G12" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="H12" s="9"/>
+      <c r="K12" s="8" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="13" s="3" customFormat="true" ht="29.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="6" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
-      <c r="H13" s="8"/>
+      <c r="H13" s="9"/>
       <c r="K13" s="3" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" s="3" customFormat="true" ht="29.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="6" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
-      <c r="H14" s="8"/>
+      <c r="H14" s="9"/>
       <c r="K14" s="3" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" s="3" customFormat="true" ht="29.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="6" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
-      <c r="H15" s="8"/>
+      <c r="H15" s="9"/>
       <c r="K15" s="3" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" s="3" customFormat="true" ht="29.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="6" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
       <c r="F16" s="0"/>
-      <c r="H16" s="8"/>
+      <c r="H16" s="9"/>
       <c r="K16" s="0"/>
       <c r="L16" s="0"/>
     </row>
     <row r="17" s="3" customFormat="true" ht="29.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="6" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
-      <c r="H17" s="8"/>
+      <c r="H17" s="9"/>
     </row>
     <row r="18" s="3" customFormat="true" ht="29.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="6" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
-      <c r="H18" s="8"/>
+      <c r="H18" s="9"/>
     </row>
     <row r="19" s="3" customFormat="true" ht="29.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="6" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
-      <c r="H19" s="8"/>
+      <c r="H19" s="9"/>
     </row>
     <row r="20" s="3" customFormat="true" ht="29.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="6" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
-      <c r="H20" s="8"/>
+      <c r="H20" s="9"/>
     </row>
     <row r="21" s="3" customFormat="true" ht="29.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="6" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
-      <c r="H21" s="8"/>
+      <c r="H21" s="9"/>
     </row>
     <row r="22" s="3" customFormat="true" ht="29.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="6" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
-      <c r="H22" s="8"/>
+      <c r="H22" s="9"/>
     </row>
     <row r="23" s="3" customFormat="true" ht="29.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="6" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
-      <c r="H23" s="8"/>
+      <c r="H23" s="9"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -827,7 +891,7 @@
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="5" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>4</v>
@@ -837,212 +901,212 @@
       <c r="B4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="8"/>
-      <c r="I4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="I4" s="8"/>
       <c r="K4" s="10"/>
     </row>
     <row r="5" s="3" customFormat="true" ht="29.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" s="8"/>
-      <c r="I5" s="9"/>
+        <v>22</v>
+      </c>
+      <c r="F5" s="9"/>
+      <c r="I5" s="8"/>
       <c r="K5" s="10"/>
     </row>
     <row r="6" s="3" customFormat="true" ht="29.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="6" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="F6" s="8"/>
-      <c r="I6" s="9"/>
+        <v>68</v>
+      </c>
+      <c r="F6" s="9"/>
+      <c r="I6" s="8"/>
       <c r="K6" s="10"/>
     </row>
     <row r="7" s="3" customFormat="true" ht="29.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="6" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="F7" s="8"/>
-      <c r="I7" s="9"/>
+        <v>69</v>
+      </c>
+      <c r="F7" s="9"/>
+      <c r="I7" s="8"/>
       <c r="K7" s="10"/>
     </row>
     <row r="8" s="3" customFormat="true" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="6" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="F8" s="8"/>
-      <c r="I8" s="9"/>
+        <v>71</v>
+      </c>
+      <c r="F8" s="9"/>
+      <c r="I8" s="8"/>
       <c r="K8" s="10"/>
     </row>
     <row r="9" s="3" customFormat="true" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="6" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="F9" s="8"/>
-      <c r="I9" s="9"/>
+        <v>72</v>
+      </c>
+      <c r="F9" s="9"/>
+      <c r="I9" s="8"/>
       <c r="K9" s="10"/>
     </row>
     <row r="10" s="3" customFormat="true" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="6" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="F10" s="8"/>
-      <c r="I10" s="9"/>
+        <v>74</v>
+      </c>
+      <c r="F10" s="9"/>
+      <c r="I10" s="8"/>
       <c r="K10" s="10"/>
     </row>
     <row r="11" s="3" customFormat="true" ht="29.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="6" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="F11" s="8"/>
-      <c r="I11" s="9"/>
+        <v>75</v>
+      </c>
+      <c r="F11" s="9"/>
+      <c r="I11" s="8"/>
       <c r="K11" s="10"/>
     </row>
     <row r="12" s="3" customFormat="true" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="6" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="F12" s="8"/>
-      <c r="I12" s="9"/>
+        <v>76</v>
+      </c>
+      <c r="F12" s="9"/>
+      <c r="I12" s="8"/>
       <c r="K12" s="10"/>
     </row>
     <row r="13" s="3" customFormat="true" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="6" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="F13" s="8"/>
-      <c r="I13" s="9"/>
+        <v>77</v>
+      </c>
+      <c r="F13" s="9"/>
+      <c r="I13" s="8"/>
       <c r="K13" s="10"/>
     </row>
     <row r="14" s="3" customFormat="true" ht="29.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="6" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="F14" s="8"/>
-      <c r="I14" s="9"/>
+        <v>78</v>
+      </c>
+      <c r="F14" s="9"/>
+      <c r="I14" s="8"/>
       <c r="K14" s="10"/>
     </row>
     <row r="15" s="3" customFormat="true" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="6" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="F15" s="8"/>
-      <c r="I15" s="9"/>
+        <v>79</v>
+      </c>
+      <c r="F15" s="9"/>
+      <c r="I15" s="8"/>
       <c r="K15" s="10"/>
     </row>
     <row r="16" s="3" customFormat="true" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="6" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="F16" s="8"/>
-      <c r="I16" s="9"/>
+        <v>80</v>
+      </c>
+      <c r="F16" s="9"/>
+      <c r="I16" s="8"/>
       <c r="K16" s="10"/>
     </row>
     <row r="17" s="3" customFormat="true" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="6" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="F17" s="8"/>
-      <c r="I17" s="9"/>
+        <v>81</v>
+      </c>
+      <c r="F17" s="9"/>
+      <c r="I17" s="8"/>
       <c r="K17" s="10"/>
     </row>
     <row r="18" s="3" customFormat="true" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="6" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="D18" s="0"/>
-      <c r="F18" s="8"/>
-      <c r="I18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="I18" s="8"/>
       <c r="K18" s="10"/>
     </row>
     <row r="19" s="3" customFormat="true" ht="29.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="F19" s="8"/>
-      <c r="I19" s="9"/>
+        <v>62</v>
+      </c>
+      <c r="F19" s="9"/>
+      <c r="I19" s="8"/>
       <c r="K19" s="10"/>
     </row>
     <row r="20" s="3" customFormat="true" ht="29.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="F20" s="8"/>
-      <c r="I20" s="9"/>
+        <v>63</v>
+      </c>
+      <c r="F20" s="9"/>
+      <c r="I20" s="8"/>
       <c r="K20" s="10"/>
     </row>
     <row r="21" s="3" customFormat="true" ht="29.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F21" s="8"/>
-      <c r="I21" s="9"/>
+        <v>64</v>
+      </c>
+      <c r="F21" s="9"/>
+      <c r="I21" s="8"/>
       <c r="K21" s="10"/>
     </row>
     <row r="22" s="3" customFormat="true" ht="29.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="F22" s="8"/>
-      <c r="I22" s="9"/>
+        <v>65</v>
+      </c>
+      <c r="F22" s="9"/>
+      <c r="I22" s="8"/>
       <c r="K22" s="10"/>
     </row>
     <row r="23" s="3" customFormat="true" ht="29.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="F23" s="8"/>
-      <c r="I23" s="9"/>
+        <v>66</v>
+      </c>
+      <c r="F23" s="9"/>
+      <c r="I23" s="8"/>
       <c r="K23" s="10"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added config move -> site
</commit_message>
<xml_diff>
--- a/.tasks/TaskJuggle.xlsx
+++ b/.tasks/TaskJuggle.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="89">
   <si>
     <t xml:space="preserve">Category</t>
   </si>
@@ -38,7 +38,13 @@
     <t xml:space="preserve">Release / Install</t>
   </si>
   <si>
-    <t xml:space="preserve">Config move</t>
+    <t xml:space="preserve">Config move back</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Config 2 move back</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Config move site</t>
   </si>
   <si>
     <t xml:space="preserve">Site: View gallery</t>
@@ -82,6 +88,9 @@
     <t xml:space="preserve">Repair Zone: image Db first element</t>
   </si>
   <si>
+    <t xml:space="preserve">Remove first tab in RSG sytem config view</t>
+  </si>
+  <si>
     <t xml:space="preserve">b) Image editor </t>
   </si>
   <si>
@@ -110,6 +119,9 @@
     <t xml:space="preserve">Copy old to new configuration data ==&gt; Test</t>
   </si>
   <si>
+    <t xml:space="preserve">Update config links to System RSG2 config</t>
+  </si>
+  <si>
     <t xml:space="preserve">a) After upload</t>
   </si>
   <si>
@@ -248,13 +260,22 @@
     <t xml:space="preserve">End of develop</t>
   </si>
   <si>
+    <t xml:space="preserve">PHP Storm: </t>
+  </si>
+  <si>
     <t xml:space="preserve">Use JedChecker</t>
   </si>
   <si>
+    <t xml:space="preserve">Code cleanup</t>
+  </si>
+  <si>
     <t xml:space="preserve">Update change log.php</t>
   </si>
   <si>
     <t xml:space="preserve">Change log.php</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inspect code</t>
   </si>
   <si>
     <t xml:space="preserve">Update Sql files</t>
@@ -297,7 +318,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -333,6 +354,14 @@
       <charset val="1"/>
     </font>
     <font>
+      <b val="true"/>
+      <sz val="12"/>
+      <color rgb="FFBA131A"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="8"/>
       <color rgb="FF0066B3"/>
       <name val="Arial"/>
@@ -350,6 +379,13 @@
       <b val="true"/>
       <sz val="8"/>
       <color rgb="FFCE181E"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFBA131A"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -397,7 +433,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -422,23 +458,31 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -509,7 +553,7 @@
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FFBA131A"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
@@ -523,10 +567,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A3:N23"/>
+  <dimension ref="A3:P23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I6" activeCellId="0" sqref="I6"/>
+      <selection pane="topLeft" activeCell="H6" activeCellId="0" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -534,13 +578,13 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="7.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="3.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="2" width="13.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="5" style="1" width="13.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="9" style="1" width="13.89"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="22" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="5" style="1" width="13.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="13.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="11" style="1" width="13.89"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="24" style="1" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="3" s="5" customFormat="true" ht="27.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" s="5" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -563,7 +607,7 @@
       <c r="H3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="I3" s="6" t="s">
         <v>7</v>
       </c>
       <c r="J3" s="5" t="s">
@@ -581,278 +625,294 @@
       <c r="N3" s="5" t="s">
         <v>12</v>
       </c>
+      <c r="O3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="P3" s="5" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="4" s="3" customFormat="true" ht="48.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="6" t="s">
+      <c r="B4" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="C4" s="7" t="s">
         <v>16</v>
       </c>
+      <c r="D4" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>18</v>
+      </c>
       <c r="F4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="H4" s="9"/>
-      <c r="K4" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="G4" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="N4" s="10" t="s">
+      <c r="H4" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="5" s="3" customFormat="true" ht="48.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="6" t="s">
+      <c r="I4" s="9"/>
+      <c r="J4" s="10"/>
+      <c r="M4" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="N4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="P4" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="7" t="s">
+    </row>
+    <row r="5" s="3" customFormat="true" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="7" t="s">
         <v>25</v>
       </c>
+      <c r="C5" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>28</v>
+      </c>
       <c r="F5" s="3" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="H5" s="9"/>
-      <c r="K5" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="L5" s="8"/>
-      <c r="N5" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="J5" s="10"/>
+      <c r="M5" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="N5" s="9"/>
+      <c r="P5" s="3" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="6" s="3" customFormat="true" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" s="6"/>
-      <c r="E6" s="8" t="s">
-        <v>32</v>
+      <c r="B6" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="7"/>
+      <c r="E6" s="9" t="s">
+        <v>36</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="H6" s="9"/>
-      <c r="K6" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="N6" s="3" t="s">
-        <v>36</v>
+        <v>38</v>
+      </c>
+      <c r="J6" s="10"/>
+      <c r="M6" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="P6" s="3" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="7" s="3" customFormat="true" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
+      <c r="B7" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
       <c r="F7" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="H7" s="9"/>
-      <c r="K7" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="L7" s="0"/>
-      <c r="N7" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
+      </c>
+      <c r="J7" s="10"/>
+      <c r="M7" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="N7" s="0"/>
+      <c r="P7" s="3" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="8" s="3" customFormat="true" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
+      <c r="B8" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
       <c r="F8" s="0"/>
       <c r="G8" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="H8" s="9"/>
-      <c r="K8" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="L8" s="0"/>
+        <v>47</v>
+      </c>
+      <c r="J8" s="10"/>
+      <c r="M8" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="N8" s="0"/>
     </row>
     <row r="9" s="3" customFormat="true" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
+      <c r="B9" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
       <c r="F9" s="0"/>
       <c r="G9" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="H9" s="9"/>
-      <c r="K9" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="L9" s="0"/>
+        <v>50</v>
+      </c>
+      <c r="J9" s="10"/>
+      <c r="M9" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="N9" s="0"/>
     </row>
     <row r="10" s="3" customFormat="true" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
+      <c r="B10" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
       <c r="E10" s="3" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="H10" s="9"/>
-      <c r="K10" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="L10" s="0"/>
+        <v>54</v>
+      </c>
+      <c r="J10" s="10"/>
+      <c r="M10" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="N10" s="0"/>
     </row>
     <row r="11" s="3" customFormat="true" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
+      <c r="B11" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
       <c r="G11" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="H11" s="9"/>
-      <c r="K11" s="0"/>
+        <v>57</v>
+      </c>
+      <c r="J11" s="10"/>
+      <c r="M11" s="0"/>
     </row>
     <row r="12" s="3" customFormat="true" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
+      <c r="B12" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
       <c r="G12" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="H12" s="9"/>
-      <c r="K12" s="0"/>
+        <v>59</v>
+      </c>
+      <c r="J12" s="10"/>
+      <c r="M12" s="0"/>
     </row>
     <row r="13" s="3" customFormat="true" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="H13" s="9"/>
-      <c r="K13" s="0"/>
+      <c r="B13" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="G13" s="0"/>
+      <c r="H13" s="0"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="10"/>
+      <c r="M13" s="0"/>
     </row>
     <row r="14" s="3" customFormat="true" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="H14" s="9"/>
-      <c r="K14" s="0"/>
+      <c r="B14" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="J14" s="10"/>
+      <c r="M14" s="0"/>
     </row>
     <row r="15" s="3" customFormat="true" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="H15" s="9"/>
-      <c r="K15" s="0"/>
-    </row>
-    <row r="16" s="3" customFormat="true" ht="29.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
+      <c r="B15" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="J15" s="10"/>
+      <c r="M15" s="0"/>
+    </row>
+    <row r="16" s="3" customFormat="true" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
       <c r="F16" s="0"/>
-      <c r="H16" s="9"/>
-      <c r="K16" s="0"/>
-      <c r="L16" s="0"/>
-    </row>
-    <row r="17" s="3" customFormat="true" ht="29.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="H17" s="9"/>
-    </row>
-    <row r="18" s="3" customFormat="true" ht="29.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="H18" s="9"/>
-    </row>
-    <row r="19" s="3" customFormat="true" ht="29.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="H19" s="9"/>
-    </row>
-    <row r="20" s="3" customFormat="true" ht="29.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="H20" s="9"/>
-    </row>
-    <row r="21" s="3" customFormat="true" ht="29.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="6" t="s">
+      <c r="J16" s="10"/>
+      <c r="M16" s="0"/>
+      <c r="N16" s="0"/>
+    </row>
+    <row r="17" s="3" customFormat="true" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="H21" s="9"/>
-    </row>
-    <row r="22" s="3" customFormat="true" ht="29.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="6" t="s">
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="J17" s="10"/>
+    </row>
+    <row r="18" s="3" customFormat="true" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="H22" s="9"/>
-    </row>
-    <row r="23" s="3" customFormat="true" ht="29.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="6" t="s">
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="J18" s="10"/>
+    </row>
+    <row r="19" s="3" customFormat="true" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="H23" s="9"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="J19" s="10"/>
+    </row>
+    <row r="20" s="3" customFormat="true" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="J20" s="10"/>
+    </row>
+    <row r="21" s="3" customFormat="true" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="J21" s="10"/>
+    </row>
+    <row r="22" s="3" customFormat="true" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="J22" s="10"/>
+    </row>
+    <row r="23" s="3" customFormat="true" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="J23" s="10"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -870,245 +930,254 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A3:K23"/>
+  <dimension ref="A3:L23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H8" activeCellId="0" sqref="H8"/>
+      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="4.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="3" style="1" width="13.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="7" style="1" width="13.89"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="19" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="3" style="1" width="13.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="8" style="1" width="13.89"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="20" style="1" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="3" s="5" customFormat="true" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="11" t="s">
+    <row r="3" s="5" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="13" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" s="3" customFormat="true" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="10"/>
+      <c r="J4" s="9"/>
+      <c r="L4" s="11"/>
+    </row>
+    <row r="5" s="3" customFormat="true" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" s="10"/>
+      <c r="J5" s="9"/>
+      <c r="L5" s="11"/>
+    </row>
+    <row r="6" s="3" customFormat="true" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G6" s="10"/>
+      <c r="J6" s="9"/>
+      <c r="L6" s="11"/>
+    </row>
+    <row r="7" s="3" customFormat="true" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="G7" s="10"/>
+      <c r="J7" s="9"/>
+      <c r="L7" s="11"/>
+    </row>
+    <row r="8" s="3" customFormat="true" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="G8" s="10"/>
+      <c r="J8" s="9"/>
+      <c r="L8" s="11"/>
+    </row>
+    <row r="9" s="3" customFormat="true" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="G9" s="10"/>
+      <c r="J9" s="9"/>
+      <c r="L9" s="11"/>
+    </row>
+    <row r="10" s="3" customFormat="true" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="G10" s="10"/>
+      <c r="J10" s="9"/>
+      <c r="L10" s="11"/>
+    </row>
+    <row r="11" s="3" customFormat="true" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="G11" s="10"/>
+      <c r="J11" s="9"/>
+      <c r="L11" s="11"/>
+    </row>
+    <row r="12" s="3" customFormat="true" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="G12" s="10"/>
+      <c r="J12" s="9"/>
+      <c r="L12" s="11"/>
+    </row>
+    <row r="13" s="3" customFormat="true" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="G13" s="10"/>
+      <c r="J13" s="9"/>
+      <c r="L13" s="11"/>
+    </row>
+    <row r="14" s="3" customFormat="true" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="G14" s="10"/>
+      <c r="J14" s="9"/>
+      <c r="L14" s="11"/>
+    </row>
+    <row r="15" s="3" customFormat="true" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G15" s="10"/>
+      <c r="J15" s="9"/>
+      <c r="L15" s="11"/>
+    </row>
+    <row r="16" s="3" customFormat="true" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="G16" s="10"/>
+      <c r="J16" s="9"/>
+      <c r="L16" s="11"/>
+    </row>
+    <row r="17" s="3" customFormat="true" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="G17" s="10"/>
+      <c r="J17" s="9"/>
+      <c r="L17" s="11"/>
+    </row>
+    <row r="18" s="3" customFormat="true" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="E18" s="0"/>
+      <c r="G18" s="10"/>
+      <c r="J18" s="9"/>
+      <c r="L18" s="11"/>
+    </row>
+    <row r="19" s="3" customFormat="true" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="G19" s="10"/>
+      <c r="J19" s="9"/>
+      <c r="L19" s="11"/>
+    </row>
+    <row r="20" s="3" customFormat="true" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="D3" s="5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" s="3" customFormat="true" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="9"/>
-      <c r="I4" s="8"/>
-      <c r="K4" s="10"/>
-    </row>
-    <row r="5" s="3" customFormat="true" ht="29.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="F5" s="9"/>
-      <c r="I5" s="8"/>
-      <c r="K5" s="10"/>
-    </row>
-    <row r="6" s="3" customFormat="true" ht="29.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" s="3" t="s">
+      <c r="G20" s="10"/>
+      <c r="J20" s="9"/>
+      <c r="L20" s="11"/>
+    </row>
+    <row r="21" s="3" customFormat="true" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="F6" s="9"/>
-      <c r="I6" s="8"/>
-      <c r="K6" s="10"/>
-    </row>
-    <row r="7" s="3" customFormat="true" ht="29.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D7" s="3" t="s">
+      <c r="G21" s="10"/>
+      <c r="J21" s="9"/>
+      <c r="L21" s="11"/>
+    </row>
+    <row r="22" s="3" customFormat="true" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="F7" s="9"/>
-      <c r="I7" s="8"/>
-      <c r="K7" s="10"/>
-    </row>
-    <row r="8" s="3" customFormat="true" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C8" s="3" t="s">
+      <c r="G22" s="10"/>
+      <c r="J22" s="9"/>
+      <c r="L22" s="11"/>
+    </row>
+    <row r="23" s="3" customFormat="true" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="F8" s="9"/>
-      <c r="I8" s="8"/>
-      <c r="K8" s="10"/>
-    </row>
-    <row r="9" s="3" customFormat="true" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="F9" s="9"/>
-      <c r="I9" s="8"/>
-      <c r="K9" s="10"/>
-    </row>
-    <row r="10" s="3" customFormat="true" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="F10" s="9"/>
-      <c r="I10" s="8"/>
-      <c r="K10" s="10"/>
-    </row>
-    <row r="11" s="3" customFormat="true" ht="29.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="F11" s="9"/>
-      <c r="I11" s="8"/>
-      <c r="K11" s="10"/>
-    </row>
-    <row r="12" s="3" customFormat="true" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="F12" s="9"/>
-      <c r="I12" s="8"/>
-      <c r="K12" s="10"/>
-    </row>
-    <row r="13" s="3" customFormat="true" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="F13" s="9"/>
-      <c r="I13" s="8"/>
-      <c r="K13" s="10"/>
-    </row>
-    <row r="14" s="3" customFormat="true" ht="29.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="F14" s="9"/>
-      <c r="I14" s="8"/>
-      <c r="K14" s="10"/>
-    </row>
-    <row r="15" s="3" customFormat="true" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="F15" s="9"/>
-      <c r="I15" s="8"/>
-      <c r="K15" s="10"/>
-    </row>
-    <row r="16" s="3" customFormat="true" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="F16" s="9"/>
-      <c r="I16" s="8"/>
-      <c r="K16" s="10"/>
-    </row>
-    <row r="17" s="3" customFormat="true" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="F17" s="9"/>
-      <c r="I17" s="8"/>
-      <c r="K17" s="10"/>
-    </row>
-    <row r="18" s="3" customFormat="true" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="D18" s="0"/>
-      <c r="F18" s="9"/>
-      <c r="I18" s="8"/>
-      <c r="K18" s="10"/>
-    </row>
-    <row r="19" s="3" customFormat="true" ht="29.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="F19" s="9"/>
-      <c r="I19" s="8"/>
-      <c r="K19" s="10"/>
-    </row>
-    <row r="20" s="3" customFormat="true" ht="29.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="F20" s="9"/>
-      <c r="I20" s="8"/>
-      <c r="K20" s="10"/>
-    </row>
-    <row r="21" s="3" customFormat="true" ht="29.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="F21" s="9"/>
-      <c r="I21" s="8"/>
-      <c r="K21" s="10"/>
-    </row>
-    <row r="22" s="3" customFormat="true" ht="29.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="F22" s="9"/>
-      <c r="I22" s="8"/>
-      <c r="K22" s="10"/>
-    </row>
-    <row r="23" s="3" customFormat="true" ht="29.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="F23" s="9"/>
-      <c r="I23" s="8"/>
-      <c r="K23" s="10"/>
+      <c r="G23" s="10"/>
+      <c r="J23" s="9"/>
+      <c r="L23" s="11"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>